<commit_message>
Git commit March 27, 2020 - Links, Fonts, redirect
</commit_message>
<xml_diff>
--- a/export_pr1.xlsx
+++ b/export_pr1.xlsx
@@ -10,7 +10,7 @@
     <sheet name="PR" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="124519" calcMode="auto" fullCalcOnLoad="0"/>
+  <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -35,10 +35,10 @@
     <t>Office/Section :</t>
   </si>
   <si>
-    <t>ORD</t>
-  </si>
-  <si>
-    <t>PR No.:  2020-0014</t>
+    <t>LGMED</t>
+  </si>
+  <si>
+    <t>PR No.:  2020-03-0160</t>
   </si>
   <si>
     <t xml:space="preserve">Date: </t>
@@ -65,14 +65,14 @@
     <t>Total Cost</t>
   </si>
   <si>
-    <t>S015</t>
-  </si>
-  <si>
-    <t>set</t>
-  </si>
-  <si>
-    <t>Regional Team Conference
-Venue and Meals (Breakfast, AM Snacks, Lunch, PM Snacks)</t>
+    <t>S863</t>
+  </si>
+  <si>
+    <t>pax</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Meals (AM Snack-Lunch-PM Snacks)
+</t>
   </si>
   <si>
     <t>Total</t>
@@ -81,7 +81,7 @@
     <t>Purpose:</t>
   </si>
   <si>
-    <t xml:space="preserve"> For the conduct of 1st Quarter Regional Team cum Planning Conference      </t>
+    <t>Meeting of the RTF ELCAC</t>
   </si>
   <si>
     <t>Requested by:</t>
@@ -96,7 +96,7 @@
     <t>Printed Name :</t>
   </si>
   <si>
-    <t>ELIAS F. FERNANDEZ, JR.</t>
+    <t>GILBERTO L. TUMAMAC</t>
   </si>
   <si>
     <t>NOEL R. BARTOLABAC, CESO V</t>
@@ -105,7 +105,7 @@
     <t>Designation :</t>
   </si>
   <si>
-    <t>OIC - Regional Director</t>
+    <t>OIC - LGMED Chief</t>
   </si>
   <si>
     <t>Assistant Regional Director</t>
@@ -1034,13 +1034,13 @@
         <v>18</v>
       </c>
       <c r="D11" s="18">
-        <v>50</v>
+        <v>110</v>
       </c>
       <c r="E11" s="26">
-        <v>1200</v>
+        <v>500</v>
       </c>
       <c r="F11" s="26">
-        <v>60000</v>
+        <v>55000</v>
       </c>
     </row>
     <row r="12" spans="1:6" customHeight="1" ht="30" s="2" customFormat="1">
@@ -1243,9 +1243,9 @@
       <c r="E36" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="F36" s="25">
+      <c r="F36" s="25" t="str">
         <f>SUM(F11:F35)</f>
-        <v>60000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:6" customHeight="1" ht="15.75">

</xml_diff>